<commit_message>
Checking the first alternate solution.
</commit_message>
<xml_diff>
--- a/CH-071 Extract from Text.xlsx
+++ b/CH-071 Extract from Text.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B84421C-8EAC-42E0-9050-76445D603F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998E83D9-F474-43F1-A647-DAE913219BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28875" yWindow="-2550" windowWidth="28410" windowHeight="24465" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
-    <sheet name="EDA2" sheetId="3" r:id="rId3"/>
+    <sheet name="Alt" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alt!$D$3:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$F$3:$F$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'EDA2'!$D$3:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$D$3:$D$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -980,6 +980,9 @@
   <wetp:taskpane dockstate="right" visibility="0" width="350" row="10">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </wetp:taskpane>
+  <wetp:taskpane dockstate="right" visibility="0" width="771" row="11">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+  </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
@@ -1010,6 +1013,27 @@
         <we:customFunctionIds>_xldudf_NUM_AI</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_NUM_WRITE</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_NUM_INFER</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
+<file path=xl/webextensions/webextension3.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{ECE817BB-2ED9-4A34-8E86-9157D6FE4DC7}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{F2BB6AA1-9536-4426-8CF3-1A9962043DAD}&quot;}"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
       </we:customFunctionIdList>
     </a:ext>
   </we:extLst>
@@ -1601,23 +1625,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04342C2B-0F8F-4DE7-937D-9263A240E973}">
-  <dimension ref="A1:D39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710DD6B6-1CFB-4222-9557-51B262EFCB7A}">
+  <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="65.19921875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="42.296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20" style="3" customWidth="1"/>
     <col min="4" max="4" width="29.69921875" style="3" customWidth="1"/>
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>28</v>
       </c>
@@ -1625,7 +1649,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1633,7 +1657,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -1642,7 +1666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="6" t="s">
         <v>17</v>
@@ -1651,7 +1675,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A5" s="2"/>
       <c r="B5" s="8" t="s">
         <v>18</v>
@@ -1660,7 +1684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A6" s="2"/>
       <c r="B6" s="6" t="s">
         <v>15</v>
@@ -1669,7 +1693,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A7" s="2"/>
       <c r="B7" s="8" t="s">
         <v>16</v>
@@ -1678,7 +1702,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
       <c r="B8" s="7" t="s">
         <v>2</v>
@@ -1687,7 +1711,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A9" s="2"/>
       <c r="B9" s="7" t="s">
         <v>3</v>
@@ -1696,7 +1720,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A10" s="2"/>
       <c r="B10" s="7" t="s">
         <v>4</v>
@@ -1705,7 +1729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A11" s="2"/>
       <c r="B11" s="7" t="s">
         <v>5</v>
@@ -1714,94 +1738,287 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:27" ht="60" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
       <c r="B12" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:27" ht="60" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
       <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:27" ht="60" x14ac:dyDescent="0.4">
       <c r="A14" s="2"/>
       <c r="B14" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:27" ht="60" x14ac:dyDescent="0.4">
       <c r="A15" s="2"/>
       <c r="B15" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:27" ht="45" x14ac:dyDescent="0.4">
       <c r="A16" s="2"/>
       <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.4">
+      <c r="C16" s="3" t="str" cm="1">
+        <f t="array" ref="C16:AA16">_xlfn.TEXTSPLIT(B16, " ")</f>
+        <v>Lastly,</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <v>we</v>
+      </c>
+      <c r="E16" s="3" t="str">
+        <v>have</v>
+      </c>
+      <c r="F16" s="3" t="str">
+        <v>made</v>
+      </c>
+      <c r="G16" s="3" t="str">
+        <v>some</v>
+      </c>
+      <c r="H16" s="3" t="str">
+        <v>updates</v>
+      </c>
+      <c r="I16" s="3" t="str">
+        <v>to</v>
+      </c>
+      <c r="J16" s="3" t="str">
+        <v>our</v>
+      </c>
+      <c r="K16" s="3" t="str">
+        <v>company</v>
+      </c>
+      <c r="L16" s="3" t="str">
+        <v>policies.</v>
+      </c>
+      <c r="M16" s="3" t="str">
+        <v>Please</v>
+      </c>
+      <c r="N16" s="3" t="str">
+        <v>review</v>
+      </c>
+      <c r="O16" s="3" t="str">
+        <v>the</v>
+      </c>
+      <c r="P16" s="3" t="str">
+        <v>revised</v>
+      </c>
+      <c r="Q16" s="3" t="str">
+        <v>documents</v>
+      </c>
+      <c r="R16" s="3" t="str">
+        <v>attached</v>
+      </c>
+      <c r="S16" s="3" t="str">
+        <v>to</v>
+      </c>
+      <c r="T16" s="3" t="str">
+        <v>this</v>
+      </c>
+      <c r="U16" s="3" t="str">
+        <v>email</v>
+      </c>
+      <c r="V16" s="3" t="str">
+        <v>and</v>
+      </c>
+      <c r="W16" s="3" t="str">
+        <v>direct</v>
+      </c>
+      <c r="X16" s="3" t="str">
+        <v>any</v>
+      </c>
+      <c r="Y16" s="3" t="str">
+        <v>questions</v>
+      </c>
+      <c r="Z16" s="3" t="str">
+        <v>to</v>
+      </c>
+      <c r="AA16" s="3" t="str">
+        <v>policy@company.com.</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="45" x14ac:dyDescent="0.4">
       <c r="A17" s="2"/>
       <c r="B17" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C17" s="3" t="str" cm="1">
+        <f t="array" ref="C17">_xlfn.TOCOL(_xlfn.IFS(1 - ISERR(FIND(".",_xlfn.ANCHORARRAY( C16)) + FIND("@",_xlfn.ANCHORARRAY( C16))),_xlfn.ANCHORARRAY( C16)), 2)</f>
+        <v>policy@company.com.</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
       <c r="B18" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C18" s="3" cm="1">
+        <f t="array" ref="C18:AA18">1-ISERR(FIND(".",_xlfn.ANCHORARRAY(C16))+FIND("@",_xlfn.ANCHORARRAY(C16))
+)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3">
+        <v>0</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>0</v>
+      </c>
+      <c r="R18" s="3">
+        <v>0</v>
+      </c>
+      <c r="S18" s="3">
+        <v>0</v>
+      </c>
+      <c r="T18" s="3">
+        <v>0</v>
+      </c>
+      <c r="U18" s="3">
+        <v>0</v>
+      </c>
+      <c r="V18" s="3">
+        <v>0</v>
+      </c>
+      <c r="W18" s="3">
+        <v>0</v>
+      </c>
+      <c r="X18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
       <c r="B19" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B21" s="3" t="str" cm="1">
+        <f t="array" ref="B21:B29">_xlfn.TOCOL(
+    _xlfn.MAP(
+        B3:B19,
+        _xlfn.LAMBDA(_xlpm.x,
+            _xlfn.LET(
+                _xlpm.y, _xlfn.TEXTSPLIT(_xlpm.x, " "),
+                _xlfn.TOCOL(_xlfn.IFS(1 - ISERR(FIND(".", _xlpm.y) + FIND("@", _xlpm.y)), _xlpm.y), 2)
+            )
+        )
+    ),
+    2
+)</f>
+        <v>sales@company.com</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A22" s="2"/>
-      <c r="B22" s="9"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B22" s="3" t="str">
+        <v>support@company.com</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B23" s="3" t="str">
+        <v>hr@company.com</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B24" s="3" t="str">
+        <v>ithelpdesk@company.com</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A25" s="2"/>
-      <c r="B25" s="9"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B25" s="3" t="str">
+        <v>events@company.com</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B26" s="3" t="str">
+        <v>recognition@company.com.</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B27" s="3" t="str">
+        <v>marketing@company.com.</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B28" s="3" t="str">
+        <v>policy@company.com.</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B29" s="3" t="str">
+        <v>john.doe@company.com</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A32" s="2"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.4">
@@ -1821,17 +2038,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{777D0607-D623-4A0C-A252-A2A2CEB17ABA}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{7BB9A54B-0F89-420C-BFE2-80A86329FA93}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{C2B65AEB-675B-4901-952F-A608A195C9C5}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{02FA1D9B-C591-4F7F-89BA-536346733839}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{3B999673-7CB4-4399-8542-8EDBF55B71F1}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{A6608F62-E378-4E24-A5A0-16EAE785E4F8}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{82654325-FF8F-4714-B35E-3164C84176E4}"/>
-    <hyperlink ref="D10" r:id="rId8" xr:uid="{80D93C05-6530-45F6-9B1C-663BD87345FF}"/>
-    <hyperlink ref="D11" r:id="rId9" xr:uid="{FCB6DFED-BA91-4D15-97D1-4357671601A2}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{CA05EB0B-F5A7-4B6D-8496-DBADB1DEA230}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{7F291212-9DDF-4723-BD55-5B2A2E1E4065}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{8A49B1FD-2F39-4839-9149-96DA13C29585}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{98A4FEAF-3920-427F-A46B-4B9D7A51B355}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{4E4A4E9D-19D3-495D-8EB5-98B0326D97A7}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{CF723099-CCB6-4CD4-B87E-F17B2F537C21}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{78A7E570-C1D9-43F3-B3E8-CE7354C001FE}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{BB94D3F4-3725-47EE-9C83-2E65AA603C5D}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{A092D880-D7D8-4A29-ADB2-06EAE5946670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2BB6AA1-9536-4426-8CF3-1A9962043DAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Found problem with the alternate solution.
</commit_message>
<xml_diff>
--- a/CH-071 Extract from Text.xlsx
+++ b/CH-071 Extract from Text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998E83D9-F474-43F1-A647-DAE913219BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA60DBCB-DD91-4DC9-9AC1-550CDC58405E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28875" yWindow="-2550" windowWidth="28410" windowHeight="24465" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="33">
   <si>
     <t>Text</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>([a-zA-Z0-9+._-]+@[a-zA-Z0-9._-]+\.[a-zA-Z0-9_-]+)</t>
+  </si>
+  <si>
+    <t>Erroneously included period at the end</t>
   </si>
 </sst>
 </file>
@@ -980,7 +983,7 @@
   <wetp:taskpane dockstate="right" visibility="0" width="350" row="10">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </wetp:taskpane>
-  <wetp:taskpane dockstate="right" visibility="0" width="771" row="11">
+  <wetp:taskpane dockstate="right" visibility="0" width="464" row="11">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1628,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710DD6B6-1CFB-4222-9557-51B262EFCB7A}">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -1942,14 +1945,57 @@
       <c r="B19" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="C19" s="3" t="str" cm="1">
+        <f t="array" ref="C19:G19">_xlfn.TEXTSPLIT(B19, " ")</f>
+        <v>John</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <v>Doe</v>
+      </c>
+      <c r="E19" s="3" t="str">
+        <v>Communications</v>
+      </c>
+      <c r="F19" s="3" t="str">
+        <v>Manager</v>
+      </c>
+      <c r="G19" s="3" t="str">
+        <v>john.doe@company.com</v>
+      </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A20" s="2"/>
+      <c r="C20" s="3" t="str" cm="1">
+        <f t="array" ref="C20">_xlfn.TOCOL(_xlfn.IFS(1 - ISERR(FIND(".",_xlfn.ANCHORARRAY( C19)) + FIND("@",_xlfn.ANCHORARRAY( C19))),_xlfn.ANCHORARRAY( C19)), 2)</f>
+        <v>john.doe@company.com</v>
+      </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A21" s="2"/>
-      <c r="B21" s="3" t="str" cm="1">
-        <f t="array" ref="B21:B29">_xlfn.TOCOL(
+      <c r="C21" s="3" cm="1">
+        <f t="array" ref="C21:G21">1-ISERR(FIND(".",_xlfn.ANCHORARRAY(C19))+FIND("@",_xlfn.ANCHORARRAY(C19))
+)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3" t="str" cm="1">
+        <f t="array" ref="B23:B31">_xlfn.TOCOL(
     _xlfn.MAP(
         B3:B19,
         _xlfn.LAMBDA(_xlpm.x,
@@ -1963,60 +2009,99 @@
 )</f>
         <v>sales@company.com</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3" t="str">
-        <v>support@company.com</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3" t="str">
-        <v>hr@company.com</v>
+      <c r="C23" s="3" t="b">
+        <f>B23=D3</f>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="str">
-        <v>ithelpdesk@company.com</v>
+        <v>support@company.com</v>
+      </c>
+      <c r="C24" s="3" t="b">
+        <f t="shared" ref="C24:C31" si="0">B24=D4</f>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="str">
-        <v>events@company.com</v>
+        <v>hr@company.com</v>
+      </c>
+      <c r="C25" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="str">
-        <v>recognition@company.com.</v>
+        <v>ithelpdesk@company.com</v>
+      </c>
+      <c r="C26" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A27" s="2"/>
       <c r="B27" s="3" t="str">
-        <v>marketing@company.com.</v>
+        <v>events@company.com</v>
+      </c>
+      <c r="C27" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A28" s="2"/>
       <c r="B28" s="3" t="str">
-        <v>policy@company.com.</v>
+        <v>recognition@company.com.</v>
+      </c>
+      <c r="C28" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="str">
-        <v>john.doe@company.com</v>
+        <v>marketing@company.com.</v>
+      </c>
+      <c r="C29" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A30" s="2"/>
+      <c r="B30" s="3" t="str">
+        <v>policy@company.com.</v>
+      </c>
+      <c r="C30" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A31" s="2"/>
+      <c r="B31" s="3" t="str">
+        <v>john.doe@company.com</v>
+      </c>
+      <c r="C31" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A32" s="2"/>

</xml_diff>

<commit_message>
Al3 simple approach, kind of useful.
</commit_message>
<xml_diff>
--- a/CH-071 Extract from Text.xlsx
+++ b/CH-071 Extract from Text.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068751E3-AA64-4C84-AFDC-65DD85034B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EDB210-D420-4D85-B30E-72356CD326BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28875" yWindow="-2550" windowWidth="28410" windowHeight="24465" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28875" yWindow="-2550" windowWidth="28410" windowHeight="24465" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt" sheetId="4" r:id="rId3"/>
     <sheet name="Alt2" sheetId="6" r:id="rId4"/>
+    <sheet name="Alt3" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alt!$D$3:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$D$3:$D$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Alt3'!$D$3:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$F$3:$F$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$D$3:$D$5</definedName>
   </definedNames>
@@ -67,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="37">
   <si>
     <t>Text</t>
   </si>
@@ -172,6 +174,12 @@
   </si>
   <si>
     <t>This is the kind of solution I would come up with.</t>
+  </si>
+  <si>
+    <t>Assumes length constraint on name.</t>
+  </si>
+  <si>
+    <t>Nice solution for ".com." problem.</t>
   </si>
 </sst>
 </file>
@@ -991,7 +999,7 @@
   <wetp:taskpane dockstate="right" visibility="0" width="350" row="10">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </wetp:taskpane>
-  <wetp:taskpane dockstate="right" visibility="0" width="379" row="11">
+  <wetp:taskpane dockstate="right" visibility="0" width="810" row="11">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -2150,7 +2158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18475B0C-A55F-4FC7-95B3-5ADB2ABA5672}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -2458,6 +2466,288 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE5E36F-532B-45F2-86C2-5C7AB83B2856}">
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="4.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="65.19921875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="20" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.69921875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.4">
+      <c r="A13" s="2"/>
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.4">
+      <c r="A15" s="2"/>
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(B16, "com.", "com"), " ", REPT(" ", 50))</f>
+        <v>Lastly,                                                  we                                                  have                                                  made                                                  some                                                  updates                                                  to                                                  our                                                  company                                                  policies.                                                  Please                                                  review                                                  the                                                  revised                                                  documents                                                  attached                                                  to                                                  this                                                  email                                                  and                                                  direct                                                  any                                                  questions                                                  to                                                  policy@company.com</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.4">
+      <c r="A17" s="2"/>
+      <c r="B17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="3" t="str" cm="1">
+        <f t="array" ref="C17">_xlfn.TOCOL(TRIM(MID(_xlfn.ANCHORARRAY(C16), FIND("@c",_xlfn.ANCHORARRAY( C16)) - 15, 50)), 2)</f>
+        <v>policy@company.com</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" s="2"/>
+      <c r="B18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="3" t="str" cm="1">
+        <f t="array" ref="C18">MID(_xlfn.ANCHORARRAY(C16), FIND("@c",_xlfn.ANCHORARRAY( C16)) - 15, 50)</f>
+        <v xml:space="preserve">         policy@company.com</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19" s="2"/>
+      <c r="B19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21" s="2"/>
+      <c r="B21" s="8" t="str" cm="1">
+        <f t="array" ref="B21:B29">_xlfn.LET(
+    _xlpm.t, SUBSTITUTE(SUBSTITUTE(B3:B19, "com.", "com"), " ", REPT(" ", 50)),
+    _xlfn.TOCOL(TRIM(MID(_xlpm.t, FIND("@c", _xlpm.t) - 15, 50)), 2)
+)</f>
+        <v>sales@company.com</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22" s="2"/>
+      <c r="B22" s="9" t="str">
+        <v>support@company.com</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23" s="2"/>
+      <c r="B23" s="9" t="str">
+        <v>hr@company.com</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24" s="2"/>
+      <c r="B24" s="8" t="str">
+        <v>ithelpdesk@company.com</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" s="2"/>
+      <c r="B25" s="9" t="str">
+        <v>events@company.com</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" s="2"/>
+      <c r="B26" s="8" t="str">
+        <v>recognition@company.com</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" s="2"/>
+      <c r="B27" s="8" t="str">
+        <v>marketing@company.com</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28" s="2"/>
+      <c r="B28" s="8" t="str">
+        <v>policy@company.com</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29" s="2"/>
+      <c r="B29" s="8" t="str">
+        <v>john.doe@company.com</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{ABC3F0DB-2A46-406B-849F-D118C4971DAC}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{E9D3290F-D683-4B56-AC55-D5D18A8BCC0A}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{F6ACE1D5-DD53-4A3D-B2D0-73398A561F31}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{1CC389E0-7057-4758-B314-666163D740EA}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{C7C19103-B9E0-4488-95F8-3D06A788B9B8}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{FDB62B07-99D6-42A7-B151-C14C89747C9F}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{502AB6DB-85CF-43F9-88FC-3C1DBBE23B6B}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{47DD835C-5D88-4DC8-9036-8EB426ED50E8}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{17FDA17B-5063-4CD8-BEA0-A44F7F055218}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
 </file>

</xml_diff>

<commit_message>
Made a lambda that will catch quite a few email addresses.
</commit_message>
<xml_diff>
--- a/CH-071 Extract from Text.xlsx
+++ b/CH-071 Extract from Text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EDB210-D420-4D85-B30E-72356CD326BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A9B422-CD56-45B0-92C0-79DAC8216675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28875" yWindow="-2550" windowWidth="28410" windowHeight="24465" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28440" yWindow="-2115" windowWidth="28410" windowHeight="24465" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,16 @@
     <sheet name="Alt" sheetId="4" r:id="rId3"/>
     <sheet name="Alt2" sheetId="6" r:id="rId4"/>
     <sheet name="Alt3" sheetId="7" r:id="rId5"/>
+    <sheet name="MySingleFunction" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alt!$D$3:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$D$3:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Alt3'!$D$3:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$F$3:$F$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">MySingleFunction!$D$3:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$D$3:$D$5</definedName>
+    <definedName name="fEmail">_xlfn.LAMBDA(_xlpm.t, _xlfn.LET( _xlpm.l,_xlfn.TEXTSPLIT(_xlpm.t,," "), _xlpm.z,_xlfn._xlws.FILTER(_xlpm.l,NOT(ISNA(_xlfn.IFS(1 - ISERR(FIND(".", _xlpm.l) + FIND("@", _xlpm.l)), _xlpm.l)))), IFERROR(IF(RIGHT(_xlpm.z,1)=".",_xlfn.TEXTBEFORE(_xlpm.z,".",-1),_xlpm.z),"") ))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="38">
   <si>
     <t>Text</t>
   </si>
@@ -180,6 +183,9 @@
   </si>
   <si>
     <t>Nice solution for ".com." problem.</t>
+  </si>
+  <si>
+    <t>I would like to make a lambda function that extracts ALL the email addresses.</t>
   </si>
 </sst>
 </file>
@@ -321,7 +327,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="4" fontId="8" fillId="0" borderId="2" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1027,6 +1033,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_NUM_AI</we:customFunctionIds>
@@ -1050,6 +1059,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1364,7 +1376,7 @@
         <v>support@company.com</v>
       </c>
       <c r="E4" s="3" t="b">
-        <f t="shared" ref="E4:E19" si="0">D4=F4</f>
+        <f t="shared" ref="E4:E11" si="0">D4=F4</f>
         <v>1</v>
       </c>
       <c r="F4" s="10" t="s">
@@ -1648,7 +1660,7 @@
   <dimension ref="A1:AA39"/>
   <sheetViews>
     <sheetView topLeftCell="B12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2159,7 +2171,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2470,8 +2482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE5E36F-532B-45F2-86C2-5C7AB83B2856}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -2748,6 +2760,315 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14B14D8-6C8F-4197-8083-7068FE55022E}">
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="4.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="65.19921875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="26.3984375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.69921875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="str" cm="1">
+        <f t="array" ref="C3:C11">_xlfn.LET(_xlpm.z,_xlfn.MAP(B3:B19,_xlfn.LAMBDA(_xlpm.t,fEmail(_xlpm.t))),_xlfn._xlws.FILTER(_xlpm.z,LEN(_xlpm.z)&gt;0))</f>
+        <v>sales@company.com</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <f>C3=D3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="10" t="str">
+        <v>support@company.com</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="b">
+        <f t="shared" ref="E4:E19" si="0">C4=D4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="10" t="str">
+        <v>hr@company.com</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="10" t="str">
+        <v>ithelpdesk@company.com</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="10" t="str">
+        <v>events@company.com</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="10" t="str">
+        <v>recognition@company.com</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="10" t="str">
+        <v>marketing@company.com</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="10" t="str">
+        <v>policy@company.com</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="10" t="str">
+        <v>john.doe@company.com</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.4">
+      <c r="A13" s="2"/>
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.4">
+      <c r="A15" s="2"/>
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.4">
+      <c r="A16" s="2"/>
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.4">
+      <c r="A17" s="2"/>
+      <c r="B17" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="2"/>
+      <c r="B18" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="2"/>
+      <c r="B19" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" s="2"/>
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" s="2"/>
+      <c r="B23" s="9" t="str" cm="1">
+        <f t="array" ref="B23">_xlfn.LAMBDA(_xlpm.t, _xlfn.LET(
+_xlpm.l,_xlfn.TEXTSPLIT(_xlpm.t,," "),
+_xlpm.z,_xlfn._xlws.FILTER(_xlpm.l,NOT(ISNA(_xlfn.IFS(1 - ISERR(FIND(".", _xlpm.l) + FIND("@", _xlpm.l)), _xlpm.l)))),
+IFERROR(IF(RIGHT(_xlpm.z,1)=".",_xlfn.TEXTBEFORE(_xlpm.z,".",-1),_xlpm.z),"")
+))(B14)</f>
+        <v>recognition@company.com</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="2"/>
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{93488941-69DB-433D-BAC5-D1EE41ACA665}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{CD19CE5B-E83E-44F9-A67D-B0D60C2FABB2}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{370DC50B-00FA-4F3C-B9B2-6E9921A9CC09}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{6F8108DD-274E-4AB7-874D-E18F35CA065D}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{AF8BA51F-8EC3-493D-BE87-616004439022}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{899DD359-9AF6-470B-BC5E-F05A4BCE7C52}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{D7A064E4-7113-4FFA-B188-CA5E9311D4C5}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{AE6A15CA-115E-45FB-B508-0685A5820F74}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{81ECAABD-731F-444B-8D29-37D0A37A6B02}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
 </file>

</xml_diff>

<commit_message>
Tested my function with ChatGPT test data
</commit_message>
<xml_diff>
--- a/CH-071 Extract from Text.xlsx
+++ b/CH-071 Extract from Text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5C92FE-A092-4311-8F1B-70583BA0566D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C223DBC-C959-4399-86DF-226127654743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="50">
   <si>
     <t>Text</t>
   </si>
@@ -188,6 +188,42 @@
   </si>
   <si>
     <t>I would like to make a lambda function that extracts ALL the email addresses.</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, john.doe@example.com consectetur adipiscing elit. Nullam ac justo nec elit tincidunt ultrices. Sed euismod, ante at bibendum mattis, augue nunc vehicula purus, vel lacinia nisl elit at libero. Fusce euismod urna at odio varius, jane.smith@emailprovider.com eget venenatis metus tincidunt. Vivamus euismod, mauris at cursus bibendum, odio libero aliquet elit, id suscipit odio elit vel libero. Sed euismod, ante at alexander.johnson@domain.net bibendum mattis, augue nunc vehicula purus, vel lacinia nisl elit at libero. Fusce euismod emily.brown@emailservice.org urna at odio varius, eget sam.wilson@company.co venenatis metus tincidunt. Vivamus david.clark@provider.net euismod, mauris at sarah.harris@emailhosting.org cursus bibendum, odio libero aliquet elit, id suscipit odio elit vel libero. Sed lisa.miller@webmail.com euismod, ante at bibendum mattis, augue nunc kevin.rogers@domain.co.uk vehicula purus, vel anna.green@emailservice.net lacinia nisl elit at libero. Fusce michael.baker@webmail.co euismod urna at odio varius, eget venenatis metus tincidunt. Vivamus euismod, mauris at cursus bibendum, odio libero aliquet elit, id suscipit odio elit vel libero.”</t>
+  </si>
+  <si>
+    <t>john.doe@example.com</t>
+  </si>
+  <si>
+    <t>jane.smith@emailprovider.com</t>
+  </si>
+  <si>
+    <t>alexander.johnson@domain.net</t>
+  </si>
+  <si>
+    <t>emily.brown@emailservice.org</t>
+  </si>
+  <si>
+    <t>sam.wilson@company.co</t>
+  </si>
+  <si>
+    <t>lisa.miller@webmail.com</t>
+  </si>
+  <si>
+    <t>david.clark@provider.net</t>
+  </si>
+  <si>
+    <t>sarah.harris@emailhosting.org</t>
+  </si>
+  <si>
+    <t>kevin.rogers@domain.co.uk</t>
+  </si>
+  <si>
+    <t>anna.green@emailservice.net</t>
+  </si>
+  <si>
+    <t>michael.baker@webmail.co</t>
   </si>
 </sst>
 </file>
@@ -302,7 +338,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -341,6 +377,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3075,15 +3114,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8E5E2E-AA34-43B3-AA23-27C5F1CF959E}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="65.19921875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="20" style="3" customWidth="1"/>
+    <col min="2" max="2" width="120.796875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="34.796875" style="3" customWidth="1"/>
     <col min="4" max="4" width="29.69921875" style="3" customWidth="1"/>
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
@@ -3327,8 +3366,11 @@
       <c r="A23" s="2"/>
       <c r="B23" s="9"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="175.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2"/>
+      <c r="B24" s="17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" s="2"/>
@@ -3339,35 +3381,146 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" s="2"/>
+      <c r="B27" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="3" t="str" cm="1">
+        <f t="array" ref="C27:C37">_xlfn.LAMBDA(_xlpm.t, _xlfn.LET(
+_xlpm.n, _xlfn.LAMBDA(_xlpm.t, LEN(_xlpm.t)-LEN(SUBSTITUTE(_xlpm.t,".",""))),
+_xlpm.l,_xlfn.TEXTSPLIT(_xlpm.t,," "),
+_xlpm.z,_xlfn._xlws.FILTER(_xlpm.l,NOT(ISNA(_xlfn.IFS(1 - ISERR(FIND(".", _xlpm.l) + FIND("@", _xlpm.l)), _xlpm.l)))),
+_xlpm.zz,IFERROR(IF(RIGHT(_xlpm.z,1)=".",_xlfn.TEXTBEFORE(_xlpm.z,".",-1),_xlpm.z),""),
+IF(ISNUMBER(FIND(".",_xlfn.TEXTAFTER(_xlpm.zz,"@"))),_xlpm.zz,"")
+))(B24)</f>
+        <v>john.doe@example.com</v>
+      </c>
+      <c r="D27" s="3" t="b" cm="1">
+        <f t="array" ref="D27:D37">_xlfn._xlws.SORT(B27:B37)=_xlfn._xlws.SORT(_xlfn.ANCHORARRAY(C27))</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" s="2"/>
+      <c r="B28" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="3" t="str">
+        <v>jane.smith@emailprovider.com</v>
+      </c>
+      <c r="D28" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" s="2"/>
+      <c r="B29" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="3" t="str">
+        <v>alexander.johnson@domain.net</v>
+      </c>
+      <c r="D29" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" s="2"/>
+      <c r="B30" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="3" t="str">
+        <v>emily.brown@emailservice.org</v>
+      </c>
+      <c r="D30" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" s="2"/>
+      <c r="B31" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="3" t="str">
+        <v>sam.wilson@company.co</v>
+      </c>
+      <c r="D31" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" s="2"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B32" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="3" t="str">
+        <v>david.clark@provider.net</v>
+      </c>
+      <c r="D32" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B33" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="3" t="str">
+        <v>sarah.harris@emailhosting.org</v>
+      </c>
+      <c r="D33" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" s="4"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B34" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="3" t="str">
+        <v>lisa.miller@webmail.com</v>
+      </c>
+      <c r="D34" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B35" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="3" t="str">
+        <v>kevin.rogers@domain.co.uk</v>
+      </c>
+      <c r="D35" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B36" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="3" t="str">
+        <v>anna.green@emailservice.net</v>
+      </c>
+      <c r="D36" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37" s="2"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="B37" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="3" t="str">
+        <v>michael.baker@webmail.co</v>
+      </c>
+      <c r="D37" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39" s="2"/>
     </row>
   </sheetData>

</xml_diff>